<commit_message>
add draft daily schedule
</commit_message>
<xml_diff>
--- a/docs/resources/training_schedule.xlsx
+++ b/docs/resources/training_schedule.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Dropbox\g2sq\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF205BB9-F66D-4134-8AC9-C3B13E495656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B951A052-9BAD-4127-BD36-AC0E691962A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{12B3E256-4ECB-4B9D-A88B-2486C2DE89B4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{12B3E256-4ECB-4B9D-A88B-2486C2DE89B4}"/>
   </bookViews>
   <sheets>
     <sheet name="newest" sheetId="5" r:id="rId1"/>
-    <sheet name="newer" sheetId="4" r:id="rId2"/>
-    <sheet name="new" sheetId="3" r:id="rId3"/>
+    <sheet name="new" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>Day</t>
   </si>
@@ -211,87 +210,6 @@
   </si>
   <si>
     <t xml:space="preserve">Conduct a field practice for trainees to practice the entire questionnaire, focusing on the new parts if necessary. Train relevant interviewing skills just prior. </t>
-  </si>
-  <si>
-    <t>1 3 2 0.5</t>
-  </si>
-  <si>
-    <t>1 2 2.5 1</t>
-  </si>
-  <si>
-    <t>Opening module, CAPI use, Questionnaire content, Written test</t>
-  </si>
-  <si>
-    <t>2 1 3 1</t>
-  </si>
-  <si>
-    <t>Review written test, Questionnaire content, Front-of-class interview, Written test</t>
-  </si>
-  <si>
-    <t>Review written test, Questionnaire content, Practice respondents on-site, Debrief</t>
-  </si>
-  <si>
-    <t>Review written test, Questionnaire content, Group practicing, Written test</t>
-  </si>
-  <si>
-    <t>Written test, Interviewing skills, Field practice</t>
-  </si>
-  <si>
-    <t>0.5 2 5</t>
-  </si>
-  <si>
-    <t>2 2 2 6</t>
-  </si>
-  <si>
-    <t>Debrief field practice, Questionnaire content, Group practicing, Written test</t>
-  </si>
-  <si>
-    <t>1 3 2 8</t>
-  </si>
-  <si>
-    <t>Review written test, Questionnaire content, Practice respondents on-site</t>
-  </si>
-  <si>
-    <t>Debrief, Interviewing skills, Field practice</t>
-  </si>
-  <si>
-    <t>1 1.5 11</t>
-  </si>
-  <si>
-    <t>1 2 10</t>
-  </si>
-  <si>
-    <t>2 2 2 1</t>
-  </si>
-  <si>
-    <t>Debrief field practice, Pre-interview tasks, Post-interview tasks, Fieldworker selection</t>
-  </si>
-  <si>
-    <t>Final field test, Supervisor training</t>
-  </si>
-  <si>
-    <t>7 2</t>
-  </si>
-  <si>
-    <t>Debrief final field test, Post-interview tasks, Supervisor training</t>
-  </si>
-  <si>
-    <t>Travel to the field, Data monitor training</t>
-  </si>
-  <si>
-    <t>Field start, Data monitor training</t>
-  </si>
-  <si>
-    <t>7 7</t>
-  </si>
-  <si>
-    <t>3 4 4 4</t>
-  </si>
-  <si>
-    <t>Debrief final field test, Administrative matters, Supervisor training, Data monitor training</t>
-  </si>
-  <si>
-    <t>3.5 3 2</t>
   </si>
   <si>
     <t>Written test</t>
@@ -738,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCC036C-9814-4A8A-AB84-8E52E23BFA94}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -792,7 +710,7 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="15" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C5" s="13">
         <v>1</v>
@@ -803,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C6" s="10">
         <v>1</v>
@@ -830,7 +748,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="9" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C9" s="10">
         <v>0.5</v>
@@ -841,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C10" s="13">
         <v>1</v>
@@ -868,7 +786,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="15" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C13" s="13">
         <v>0.5</v>
@@ -879,7 +797,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C14" s="10">
         <v>1</v>
@@ -917,7 +835,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C18" s="13">
         <v>0.5</v>
@@ -926,7 +844,7 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="15" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
@@ -935,7 +853,7 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="15" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C20" s="13">
         <v>4</v>
@@ -973,7 +891,7 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="9" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C24" s="10">
         <v>0.5</v>
@@ -993,7 +911,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C26" s="10">
         <v>1</v>
@@ -1020,7 +938,7 @@
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="9" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C29" s="10">
         <v>0.5</v>
@@ -1031,7 +949,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C30" s="13">
         <v>1</v>
@@ -1058,7 +976,7 @@
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
       <c r="B33" s="15" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C33" s="13">
         <v>0.5</v>
@@ -1069,7 +987,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C34" s="10">
         <v>1</v>
@@ -1107,7 +1025,7 @@
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="12"/>
       <c r="B38" s="15" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C38" s="13">
         <v>1.5</v>
@@ -1116,7 +1034,7 @@
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="B39" s="15" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C39" s="13">
         <v>4</v>
@@ -1136,7 +1054,7 @@
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="9" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C41" s="10">
         <v>2</v>
@@ -1145,7 +1063,7 @@
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="9" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C42" s="10">
         <v>2</v>
@@ -1165,14 +1083,14 @@
         <v>13</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C44" s="13"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
       <c r="B45" s="13" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C45" s="13">
         <v>2</v>
@@ -1192,7 +1110,7 @@
         <v>15</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C47" s="13">
         <v>3.5</v>
@@ -1201,7 +1119,7 @@
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
       <c r="B48" s="15" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C48" s="13">
         <v>3</v>
@@ -1210,7 +1128,7 @@
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
       <c r="B49" s="13" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C49" s="13">
         <v>2</v>
@@ -1221,14 +1139,14 @@
         <v>16</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C50" s="10"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="8"/>
       <c r="B51" s="10" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C51" s="10">
         <v>2</v>
@@ -1239,7 +1157,7 @@
         <v>17</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C52" s="13">
         <v>3</v>
@@ -1257,7 +1175,7 @@
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="12"/>
       <c r="B54" s="14" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C54" s="13">
         <v>4</v>
@@ -1332,323 +1250,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B98CB75-A936-431E-A1C5-A35BD6B20FEB}">
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="A1:C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
-    <col min="2" max="2" width="25.77734375" customWidth="1"/>
-    <col min="3" max="3" width="28.21875" customWidth="1"/>
-    <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="47.21875" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C104AE7-6CE6-4215-AB2A-D2917D7A1CE0}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Josephine's correction training plan
</commit_message>
<xml_diff>
--- a/docs/resources/training_schedule.xlsx
+++ b/docs/resources/training_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Dropbox\g2sq\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE938B72-5C6D-4049-AD91-300FE46A8E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7178C461-22BB-4836-9963-ED7E039016FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{12B3E256-4ECB-4B9D-A88B-2486C2DE89B4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>Day</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Hrs</t>
   </si>
   <si>
-    <t>Opening module</t>
-  </si>
-  <si>
     <t>CAPI use</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>Travel to the field</t>
   </si>
   <si>
-    <t>Data Monitor Training</t>
-  </si>
-  <si>
     <t>Field start</t>
   </si>
   <si>
@@ -192,6 +186,15 @@
   </si>
   <si>
     <t>16.30 - 17.00</t>
+  </si>
+  <si>
+    <t>Welcome/introduction</t>
+  </si>
+  <si>
+    <t>Data Monitor Training (in parallel)</t>
+  </si>
+  <si>
+    <t>Supervisor Training (after)</t>
   </si>
 </sst>
 </file>
@@ -318,12 +321,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -339,6 +336,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCC036C-9814-4A8A-AB84-8E52E23BFA94}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,157 +675,157 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="14">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="9" t="s">
-        <v>6</v>
       </c>
       <c r="C3" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="20">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="6">
         <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
+      <c r="A10" s="19">
         <v>3</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+      <c r="A14" s="20">
         <v>4</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="6">
         <v>2.5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="5" t="s">
         <v>3</v>
       </c>
@@ -831,36 +834,36 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="14">
+      <c r="A18" s="19">
         <v>5</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="13">
+      <c r="A21" s="20">
         <v>6</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -871,27 +874,27 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="B23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="C23" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24" s="6">
         <v>0.5</v>
@@ -907,112 +910,112 @@
       <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="13">
+      <c r="A26" s="20">
         <v>8</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C29" s="6">
         <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="14">
+      <c r="A30" s="19">
         <v>9</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C30" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C33" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="13">
+      <c r="A34" s="20">
         <v>10</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C34" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C36" s="6">
         <v>3.5</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="14">
+      <c r="A37" s="19">
         <v>11</v>
       </c>
       <c r="B37" s="10" t="s">
@@ -1023,25 +1026,25 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C38" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C39" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="13">
+      <c r="A40" s="20">
         <v>12</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -1052,45 +1055,45 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
+      <c r="A41" s="20"/>
       <c r="B41" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C41" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="13"/>
+      <c r="A42" s="20"/>
       <c r="B42" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C42" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="13"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C43" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="14">
+      <c r="A44" s="19">
         <v>13</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C44" s="8"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="14"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="8" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C45" s="8">
         <v>2</v>
@@ -1106,126 +1109,131 @@
       <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="14">
+      <c r="A47" s="19">
         <v>15</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C47" s="8">
         <v>3.5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="14"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C48" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="8" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C49" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="13">
+      <c r="A50" s="20">
         <v>16</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="20"/>
+      <c r="B51" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="19">
+        <v>17</v>
+      </c>
+      <c r="B52" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="C50" s="6"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="13"/>
-      <c r="B51" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="14">
-        <v>17</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="C52" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="14"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C53" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="14"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C54" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="14"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="9" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C55" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="13">
+      <c r="A56" s="20">
         <v>18</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C56" s="6"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="13"/>
+      <c r="A57" s="20"/>
       <c r="B57" s="6" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C57" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="14">
+      <c r="A58" s="19">
         <v>19</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C58" s="8"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="14"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="8" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C59" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A59"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
@@ -1238,11 +1246,6 @@
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1267,160 +1270,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="B2" s="16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="D2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="18" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="B3" s="18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="D3" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="B4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="20" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20" t="s">
+      <c r="B6" s="16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="C6" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B7" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B8" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B9" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="C9" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="B11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18" t="s">
-        <v>33</v>
+      <c r="B12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>